<commit_message>
Added Arrays - Exe and some updates
</commit_message>
<xml_diff>
--- a/Tech Module/00. Technology-Fundamentals-Module-Schedule.xlsx
+++ b/Tech Module/00. Technology-Fundamentals-Module-Schedule.xlsx
@@ -1852,7 +1852,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:L16"/>
+      <selection activeCell="A15" sqref="A15:L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2358,41 +2358,41 @@
       <c r="L14" s="59"/>
     </row>
     <row r="15" spans="1:12" s="7" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="39">
+      <c r="C15" s="54">
         <f t="shared" ref="C15" si="6">C12 + 4</f>
         <v>43014</v>
       </c>
-      <c r="D15" s="40" t="str">
+      <c r="D15" s="55" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
         <v>Friday</v>
       </c>
-      <c r="E15" s="41" t="str">
+      <c r="E15" s="56" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
         <v>18:00-22:00</v>
       </c>
-      <c r="F15" s="42" t="str">
+      <c r="F15" s="57" t="str">
         <f>IF(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), "Team", "Nakov")</f>
         <v>Team</v>
       </c>
-      <c r="G15" s="43">
+      <c r="G15" s="58">
         <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
         <v>43020</v>
       </c>
-      <c r="H15" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="J15" s="44"/>
-      <c r="K15" s="44"/>
-      <c r="L15" s="44"/>
+      <c r="H15" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="59"/>
+      <c r="K15" s="59"/>
+      <c r="L15" s="59"/>
     </row>
     <row r="16" spans="1:12" s="9" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A16" s="52" t="s">

</xml_diff>

<commit_message>
Added some Labs and Exercises
</commit_message>
<xml_diff>
--- a/Tech Module/00. Technology-Fundamentals-Module-Schedule.xlsx
+++ b/Tech Module/00. Technology-Fundamentals-Module-Schedule.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Software Technologies Group I" sheetId="2" r:id="rId3"/>
     <sheet name="Software Technologies Group II" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="124">
   <si>
     <t>Part I - Programming Fundamentals</t>
   </si>
@@ -388,17 +388,24 @@
   </si>
   <si>
     <t>Ivo</t>
+  </si>
+  <si>
+    <t>6.2</t>
+  </si>
+  <si>
+    <t>Arrays &amp; Methods - More Exercises</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd/mmm"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="166" formatCode="d\-mmm"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -485,6 +492,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -512,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -695,11 +715,294 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="44">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="[$-409]d\-mmm;@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="[$-409]d\-mmm;@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="d\-mmm"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="d\-mmm"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="d\-mmm"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-409]d\-mmm;@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1179,267 +1482,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="[$-409]d\-mmm;@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="[$-409]d\-mmm;@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="d\-mmm"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="d\-mmm"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="d\-mmm"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
       </font>
@@ -1479,29 +1521,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:L32" totalsRowShown="0" dataDxfId="41">
-  <autoFilter ref="A2:L32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:L33" totalsRowShown="0" dataDxfId="12">
+  <autoFilter ref="A2:L33"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="#" dataDxfId="40"/>
-    <tableColumn id="2" name="Lesson" dataDxfId="39"/>
-    <tableColumn id="3" name="Date" dataDxfId="38"/>
-    <tableColumn id="4" name="Day" dataDxfId="37">
+    <tableColumn id="1" name="#" dataDxfId="11"/>
+    <tableColumn id="2" name="Lesson" dataDxfId="10"/>
+    <tableColumn id="3" name="Date" dataDxfId="9"/>
+    <tableColumn id="4" name="Day" dataDxfId="8">
       <calculatedColumnFormula>TEXT(Table2[[#This Row],[Date]],"dddd")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Time" dataDxfId="36">
+    <tableColumn id="5" name="Time" dataDxfId="7">
       <calculatedColumnFormula>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Trainer" dataDxfId="35">
+    <tableColumn id="6" name="Trainer" dataDxfId="6">
       <calculatedColumnFormula>IF(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), "Team", "TBA")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Homework" dataDxfId="34">
+    <tableColumn id="9" name="Homework" dataDxfId="5">
       <calculatedColumnFormula>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Live" dataDxfId="33"/>
-    <tableColumn id="7" name="Certificate" dataDxfId="32"/>
-    <tableColumn id="10" name="Column1" dataDxfId="31"/>
-    <tableColumn id="11" name="Column2" dataDxfId="30"/>
-    <tableColumn id="12" name="Column3" dataDxfId="29"/>
+    <tableColumn id="8" name="Live" dataDxfId="4"/>
+    <tableColumn id="7" name="Certificate" dataDxfId="3"/>
+    <tableColumn id="10" name="Column1" dataDxfId="2"/>
+    <tableColumn id="11" name="Column2" dataDxfId="1"/>
+    <tableColumn id="12" name="Column3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1511,23 +1553,23 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A2:L32" totalsRowShown="0">
   <autoFilter ref="A2:L32"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="#" dataDxfId="28"/>
-    <tableColumn id="2" name="Lesson" dataDxfId="27"/>
-    <tableColumn id="3" name="Date" dataDxfId="26"/>
-    <tableColumn id="4" name="Day" dataDxfId="25">
+    <tableColumn id="1" name="#" dataDxfId="41"/>
+    <tableColumn id="2" name="Lesson" dataDxfId="40"/>
+    <tableColumn id="3" name="Date" dataDxfId="39"/>
+    <tableColumn id="4" name="Day" dataDxfId="38">
       <calculatedColumnFormula>TEXT(Table24[[#This Row],[Date]],"dddd")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Time" dataDxfId="24">
+    <tableColumn id="5" name="Time" dataDxfId="37">
       <calculatedColumnFormula>IF(OR(Table24[[#This Row],[Day]]="Thursday", Table24[[#This Row],[Day]]="Friday"),"18:00-22:00", IF(Table24[[#This Row],[Day]]="Saturday", "09:00-13:00", "19:00-22:00"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Trainer" dataDxfId="23">
+    <tableColumn id="6" name="Trainer" dataDxfId="36">
       <calculatedColumnFormula>IF(ISNUMBER(SEARCH("Exercises", Table24[[#This Row],[Lesson]])), "Team", "TBA")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Homework" dataDxfId="22">
+    <tableColumn id="9" name="Homework" dataDxfId="35">
       <calculatedColumnFormula>IF(OR(ISNUMBER(SEARCH("Exercises", Table24[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table24[[#This Row],[Lesson]]))), MIN(Table24[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Live" dataDxfId="21"/>
-    <tableColumn id="7" name="Certificate" dataDxfId="20"/>
+    <tableColumn id="8" name="Live" dataDxfId="34"/>
+    <tableColumn id="7" name="Certificate" dataDxfId="33"/>
     <tableColumn id="10" name="Column1"/>
     <tableColumn id="11" name="Column2"/>
     <tableColumn id="12" name="Column3"/>
@@ -1537,24 +1579,24 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table27" displayName="Table27" ref="A2:J40" totalsRowShown="0" headerRowDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table27" displayName="Table27" ref="A2:J40" totalsRowShown="0" headerRowDxfId="32">
   <autoFilter ref="A2:J40"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="#" dataDxfId="18"/>
-    <tableColumn id="2" name="Lesson" dataDxfId="17"/>
-    <tableColumn id="3" name="Date" dataDxfId="16"/>
-    <tableColumn id="4" name="Day" dataDxfId="15">
+    <tableColumn id="1" name="#" dataDxfId="31"/>
+    <tableColumn id="2" name="Lesson" dataDxfId="30"/>
+    <tableColumn id="3" name="Date" dataDxfId="29"/>
+    <tableColumn id="4" name="Day" dataDxfId="28">
       <calculatedColumnFormula>TEXT(C3,"dddd")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Time" dataDxfId="14">
+    <tableColumn id="5" name="Time" dataDxfId="27">
       <calculatedColumnFormula>IF(OR(D3="Monday", D3="Wednesday", D3="Thursday"),"14:00-18:00","18:00-22:00")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Trainer" dataDxfId="13">
+    <tableColumn id="6" name="Trainer" dataDxfId="26">
       <calculatedColumnFormula>IF(OR(D3="Monday", D3="Wednesday"),"Nakov","Team")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Homework" dataDxfId="12"/>
-    <tableColumn id="8" name="Live" dataDxfId="11"/>
-    <tableColumn id="7" name="Certificate" dataDxfId="10" dataCellStyle="Normal"/>
+    <tableColumn id="9" name="Homework" dataDxfId="25"/>
+    <tableColumn id="8" name="Live" dataDxfId="24"/>
+    <tableColumn id="7" name="Certificate" dataDxfId="23" dataCellStyle="Normal"/>
     <tableColumn id="10" name="Lab"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1562,24 +1604,24 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table278" displayName="Table278" ref="A2:J39" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table278" displayName="Table278" ref="A2:J39" totalsRowShown="0" headerRowDxfId="22">
   <autoFilter ref="A2:J39"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="#" dataDxfId="8"/>
-    <tableColumn id="2" name="Lesson" dataDxfId="7"/>
-    <tableColumn id="3" name="Date" dataDxfId="6"/>
-    <tableColumn id="4" name="Day" dataDxfId="5">
+    <tableColumn id="1" name="#" dataDxfId="21"/>
+    <tableColumn id="2" name="Lesson" dataDxfId="20"/>
+    <tableColumn id="3" name="Date" dataDxfId="19"/>
+    <tableColumn id="4" name="Day" dataDxfId="18">
       <calculatedColumnFormula>TEXT(C3,"dddd")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Time" dataDxfId="4">
+    <tableColumn id="5" name="Time" dataDxfId="17">
       <calculatedColumnFormula>IF(OR(D3="Wednesday", D3="Thursday", D3="Friday"),"18:00-22:00", IF(D3="Saturday", "09:00-13:00", "19:00-22:00"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Trainer" dataDxfId="3">
+    <tableColumn id="6" name="Trainer" dataDxfId="16">
       <calculatedColumnFormula>IF(OR(D3="Monday", D3="Wednesday"),"Nakov","Team")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Homework" dataDxfId="2"/>
-    <tableColumn id="8" name="Live" dataDxfId="1"/>
-    <tableColumn id="7" name="Certificate" dataDxfId="0" dataCellStyle="Normal"/>
+    <tableColumn id="9" name="Homework" dataDxfId="15"/>
+    <tableColumn id="8" name="Live" dataDxfId="14"/>
+    <tableColumn id="7" name="Certificate" dataDxfId="13" dataCellStyle="Normal"/>
     <tableColumn id="10" name="Lab"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1849,10 +1891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:L15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1930,11 +1972,11 @@
       </c>
       <c r="D3" s="40" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Monday</v>
+        <v>понеделник</v>
       </c>
       <c r="E3" s="41" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
-        <v>13:30-17:30</v>
+        <v>18:00-22:00</v>
       </c>
       <c r="F3" s="42" t="s">
         <v>121</v>
@@ -1965,11 +2007,11 @@
       </c>
       <c r="D4" s="55" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Monday</v>
+        <v>понеделник</v>
       </c>
       <c r="E4" s="56" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
-        <v>13:30-17:30</v>
+        <v>18:00-22:00</v>
       </c>
       <c r="F4" s="57" t="s">
         <v>121</v>
@@ -2001,7 +2043,7 @@
       </c>
       <c r="D5" s="55" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Tuesday</v>
+        <v>вторник</v>
       </c>
       <c r="E5" s="56" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
@@ -2013,7 +2055,7 @@
       </c>
       <c r="G5" s="58">
         <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
-        <v>43003</v>
+        <v>42866</v>
       </c>
       <c r="H5" s="57" t="s">
         <v>15</v>
@@ -2038,11 +2080,11 @@
       </c>
       <c r="D6" s="55" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Thursday</v>
+        <v>четвъртък</v>
       </c>
       <c r="E6" s="56" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
-        <v>13:30-17:30</v>
+        <v>18:00-22:00</v>
       </c>
       <c r="F6" s="57" t="s">
         <v>121</v>
@@ -2074,7 +2116,7 @@
       </c>
       <c r="D7" s="55" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Friday</v>
+        <v>петък</v>
       </c>
       <c r="E7" s="56" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
@@ -2086,7 +2128,7 @@
       </c>
       <c r="G7" s="58">
         <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
-        <v>43006</v>
+        <v>42866</v>
       </c>
       <c r="H7" s="57" t="s">
         <v>15</v>
@@ -2111,11 +2153,11 @@
       </c>
       <c r="D8" s="40" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Monday</v>
+        <v>понеделник</v>
       </c>
       <c r="E8" s="41" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
-        <v>13:30-17:30</v>
+        <v>18:00-22:00</v>
       </c>
       <c r="F8" s="42" t="str">
         <f>IF(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), "Team", "Nakov")</f>
@@ -2148,7 +2190,7 @@
       </c>
       <c r="D9" s="40" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Tuesday</v>
+        <v>вторник</v>
       </c>
       <c r="E9" s="41" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
@@ -2160,7 +2202,7 @@
       </c>
       <c r="G9" s="43">
         <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
-        <v>43010</v>
+        <v>42866</v>
       </c>
       <c r="H9" s="42" t="s">
         <v>15</v>
@@ -2185,11 +2227,11 @@
       </c>
       <c r="D10" s="55" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Thursday</v>
+        <v>четвъртък</v>
       </c>
       <c r="E10" s="56" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
-        <v>13:30-17:30</v>
+        <v>18:00-22:00</v>
       </c>
       <c r="F10" s="57" t="str">
         <f>IF(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), "Team", "Nakov")</f>
@@ -2222,7 +2264,7 @@
       </c>
       <c r="D11" s="40" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Friday</v>
+        <v>петък</v>
       </c>
       <c r="E11" s="41" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
@@ -2234,7 +2276,7 @@
       </c>
       <c r="G11" s="43">
         <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
-        <v>43013</v>
+        <v>42866</v>
       </c>
       <c r="H11" s="42" t="s">
         <v>15</v>
@@ -2259,11 +2301,11 @@
       </c>
       <c r="D12" s="40" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Monday</v>
+        <v>понеделник</v>
       </c>
       <c r="E12" s="41" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
-        <v>13:30-17:30</v>
+        <v>18:00-22:00</v>
       </c>
       <c r="F12" s="42" t="str">
         <f>IF(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), "Team", "Nakov")</f>
@@ -2296,7 +2338,7 @@
       </c>
       <c r="D13" s="40" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Tuesday</v>
+        <v>вторник</v>
       </c>
       <c r="E13" s="41" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
@@ -2308,7 +2350,7 @@
       </c>
       <c r="G13" s="43">
         <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
-        <v>43017</v>
+        <v>42866</v>
       </c>
       <c r="H13" s="42" t="s">
         <v>15</v>
@@ -2333,11 +2375,11 @@
       </c>
       <c r="D14" s="55" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Thursday</v>
+        <v>четвъртък</v>
       </c>
       <c r="E14" s="56" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
-        <v>13:30-17:30</v>
+        <v>18:00-22:00</v>
       </c>
       <c r="F14" s="57" t="str">
         <f>IF(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), "Team", "Nakov")</f>
@@ -2365,12 +2407,12 @@
         <v>40</v>
       </c>
       <c r="C15" s="54">
-        <f t="shared" ref="C15" si="6">C12 + 4</f>
+        <f>C12 + 4</f>
         <v>43014</v>
       </c>
       <c r="D15" s="55" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Friday</v>
+        <v>петък</v>
       </c>
       <c r="E15" s="56" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
@@ -2382,7 +2424,7 @@
       </c>
       <c r="G15" s="58">
         <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
-        <v>43020</v>
+        <v>42866</v>
       </c>
       <c r="H15" s="57" t="s">
         <v>15</v>
@@ -2395,426 +2437,419 @@
       <c r="L15" s="59"/>
     </row>
     <row r="16" spans="1:12" s="9" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="52" t="s">
+      <c r="A16" s="67" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" s="68" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" s="69"/>
+      <c r="D16" s="70" t="str">
+        <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
+        <v>събота</v>
+      </c>
+      <c r="E16" s="70" t="str">
+        <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
+        <v>18:00-22:00</v>
+      </c>
+      <c r="F16" s="71" t="str">
+        <f>IF(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), "Team", "TBA")</f>
+        <v>Team</v>
+      </c>
+      <c r="G16" s="72">
+        <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
+        <v>6</v>
+      </c>
+      <c r="H16" s="71"/>
+      <c r="I16" s="73"/>
+      <c r="J16" s="66"/>
+      <c r="K16" s="66"/>
+      <c r="L16" s="66"/>
+    </row>
+    <row r="17" spans="1:12" s="7" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="53" t="s">
+      <c r="B17" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="54">
-        <f t="shared" ref="C16" si="7">C12 + 7</f>
+      <c r="C17" s="54">
+        <f>C12 + 7</f>
         <v>43017</v>
       </c>
-      <c r="D16" s="55" t="str">
+      <c r="D17" s="55" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Monday</v>
-      </c>
-      <c r="E16" s="56" t="str">
+        <v>понеделник</v>
+      </c>
+      <c r="E17" s="56" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
-        <v>13:30-17:30</v>
-      </c>
-      <c r="F16" s="57" t="str">
+        <v>18:00-22:00</v>
+      </c>
+      <c r="F17" s="57" t="str">
         <f>IF(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), "Team", "Nakov")</f>
         <v>Nakov</v>
       </c>
-      <c r="G16" s="58" t="str">
+      <c r="G17" s="58" t="str">
         <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="H16" s="57" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="57" t="s">
-        <v>15</v>
-      </c>
-      <c r="J16" s="64"/>
-      <c r="K16" s="64"/>
-      <c r="L16" s="64"/>
-    </row>
-    <row r="17" spans="1:12" s="7" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="45" t="s">
+      <c r="H17" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="64"/>
+      <c r="K17" s="64"/>
+      <c r="L17" s="64"/>
+    </row>
+    <row r="18" spans="1:12" s="9" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B18" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="39">
-        <f t="shared" ref="C17" si="8">C16 + 1</f>
+      <c r="C18" s="39">
+        <f t="shared" ref="C18" si="6">C17 + 1</f>
         <v>43018</v>
       </c>
-      <c r="D17" s="40" t="str">
+      <c r="D18" s="40" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Tuesday</v>
-      </c>
-      <c r="E17" s="41" t="str">
+        <v>вторник</v>
+      </c>
+      <c r="E18" s="41" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
         <v>18:00-22:00</v>
       </c>
-      <c r="F17" s="42" t="str">
+      <c r="F18" s="42" t="str">
         <f>IF(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), "Team", "Nakov")</f>
         <v>Team</v>
       </c>
-      <c r="G17" s="43">
+      <c r="G18" s="43">
         <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
-        <v>43024</v>
-      </c>
-      <c r="H17" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="44"/>
-      <c r="K17" s="44"/>
-      <c r="L17" s="44"/>
-    </row>
-    <row r="18" spans="1:12" s="9" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="37" t="s">
+        <v>42866</v>
+      </c>
+      <c r="H18" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="44"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="44"/>
+    </row>
+    <row r="19" spans="1:12" s="7" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B19" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="39">
-        <f t="shared" ref="C18" si="9">C16 + 3</f>
+      <c r="C19" s="39">
+        <f t="shared" ref="C19" si="7">C17 + 3</f>
         <v>43020</v>
       </c>
-      <c r="D18" s="40" t="str">
+      <c r="D19" s="40" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Thursday</v>
-      </c>
-      <c r="E18" s="41" t="str">
+        <v>четвъртък</v>
+      </c>
+      <c r="E19" s="41" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
-        <v>13:30-17:30</v>
-      </c>
-      <c r="F18" s="42" t="str">
+        <v>18:00-22:00</v>
+      </c>
+      <c r="F19" s="42" t="str">
         <f>IF(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), "Team", "Nakov")</f>
         <v>Nakov</v>
       </c>
-      <c r="G18" s="43" t="str">
+      <c r="G19" s="43" t="str">
         <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="H18" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="J18" s="49"/>
-      <c r="K18" s="49"/>
-      <c r="L18" s="49"/>
-    </row>
-    <row r="19" spans="1:12" s="7" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="45" t="s">
+      <c r="H19" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" s="49"/>
+      <c r="K19" s="49"/>
+      <c r="L19" s="49"/>
+    </row>
+    <row r="20" spans="1:12" s="9" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="46" t="s">
+      <c r="B20" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="39">
-        <f t="shared" ref="C19" si="10">C16 + 4</f>
+      <c r="C20" s="39">
+        <f t="shared" ref="C20" si="8">C17 + 4</f>
         <v>43021</v>
       </c>
-      <c r="D19" s="40" t="str">
+      <c r="D20" s="40" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Friday</v>
-      </c>
-      <c r="E19" s="41" t="str">
+        <v>петък</v>
+      </c>
+      <c r="E20" s="41" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
         <v>18:00-22:00</v>
       </c>
-      <c r="F19" s="42" t="str">
+      <c r="F20" s="42" t="str">
         <f>IF(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), "Team", "Nakov")</f>
         <v>Team</v>
       </c>
-      <c r="G19" s="43">
+      <c r="G20" s="43">
         <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
-        <v>43027</v>
-      </c>
-      <c r="H19" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="J19" s="44"/>
-      <c r="K19" s="44"/>
-      <c r="L19" s="44"/>
-    </row>
-    <row r="20" spans="1:12" s="9" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="37" t="s">
+        <v>42866</v>
+      </c>
+      <c r="H20" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="44"/>
+      <c r="K20" s="44"/>
+      <c r="L20" s="44"/>
+    </row>
+    <row r="21" spans="1:12" s="7" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="B21" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="39">
-        <f t="shared" ref="C20" si="11">C16 + 7</f>
+      <c r="C21" s="39">
+        <f t="shared" ref="C21" si="9">C17 + 7</f>
         <v>43024</v>
       </c>
-      <c r="D20" s="40" t="str">
+      <c r="D21" s="40" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Monday</v>
-      </c>
-      <c r="E20" s="41" t="str">
+        <v>понеделник</v>
+      </c>
+      <c r="E21" s="41" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
-        <v>13:30-17:30</v>
-      </c>
-      <c r="F20" s="42" t="str">
+        <v>18:00-22:00</v>
+      </c>
+      <c r="F21" s="42" t="str">
         <f>IF(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), "Team", "Nakov")</f>
         <v>Nakov</v>
       </c>
-      <c r="G20" s="43" t="str">
+      <c r="G21" s="43" t="str">
         <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="H20" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="J20" s="49"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="49"/>
-    </row>
-    <row r="21" spans="1:12" s="7" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="45" t="s">
+      <c r="H21" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="49"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+    </row>
+    <row r="22" spans="1:12" s="9" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A22" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="46" t="s">
+      <c r="B22" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="39">
-        <f t="shared" ref="C21" si="12">C20 + 1</f>
+      <c r="C22" s="39">
+        <f t="shared" ref="C22" si="10">C21 + 1</f>
         <v>43025</v>
       </c>
-      <c r="D21" s="40" t="str">
+      <c r="D22" s="40" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Tuesday</v>
-      </c>
-      <c r="E21" s="41" t="str">
+        <v>вторник</v>
+      </c>
+      <c r="E22" s="41" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
         <v>18:00-22:00</v>
       </c>
-      <c r="F21" s="42" t="str">
+      <c r="F22" s="42" t="str">
         <f>IF(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), "Team", "Nakov")</f>
         <v>Team</v>
       </c>
-      <c r="G21" s="43">
+      <c r="G22" s="43">
         <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
-        <v>43031</v>
-      </c>
-      <c r="H21" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="J21" s="44"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="44"/>
-    </row>
-    <row r="22" spans="1:12" s="9" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="37" t="s">
+        <v>42866</v>
+      </c>
+      <c r="H22" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
+    </row>
+    <row r="23" spans="1:12" s="7" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A23" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="38" t="s">
+      <c r="B23" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="39">
-        <f t="shared" ref="C22" si="13">C20 + 3</f>
+      <c r="C23" s="39">
+        <f t="shared" ref="C23" si="11">C21 + 3</f>
         <v>43027</v>
       </c>
-      <c r="D22" s="40" t="str">
+      <c r="D23" s="40" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Thursday</v>
-      </c>
-      <c r="E22" s="41" t="str">
+        <v>четвъртък</v>
+      </c>
+      <c r="E23" s="41" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
-        <v>13:30-17:30</v>
-      </c>
-      <c r="F22" s="42" t="str">
+        <v>18:00-22:00</v>
+      </c>
+      <c r="F23" s="42" t="str">
         <f>IF(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), "Team", "Nakov")</f>
         <v>Nakov</v>
       </c>
-      <c r="G22" s="43" t="str">
+      <c r="G23" s="43" t="str">
         <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="H22" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="I22" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="J22" s="49"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="49"/>
-    </row>
-    <row r="23" spans="1:12" s="7" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="45" t="s">
+      <c r="H23" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+    </row>
+    <row r="24" spans="1:12" s="9" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="46" t="s">
+      <c r="B24" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="39">
-        <f t="shared" ref="C23" si="14">C20 + 4</f>
+      <c r="C24" s="39">
+        <f t="shared" ref="C24" si="12">C21 + 4</f>
         <v>43028</v>
       </c>
-      <c r="D23" s="40" t="str">
+      <c r="D24" s="40" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Friday</v>
-      </c>
-      <c r="E23" s="41" t="str">
+        <v>петък</v>
+      </c>
+      <c r="E24" s="41" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
         <v>18:00-22:00</v>
       </c>
-      <c r="F23" s="42" t="str">
+      <c r="F24" s="42" t="str">
         <f>IF(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), "Team", "Nakov")</f>
         <v>Team</v>
       </c>
-      <c r="G23" s="43">
+      <c r="G24" s="43">
         <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
-        <v>43034</v>
-      </c>
-      <c r="H23" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="J23" s="44"/>
-      <c r="K23" s="44"/>
-      <c r="L23" s="44"/>
-    </row>
-    <row r="24" spans="1:12" s="9" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="37" t="s">
+        <v>42866</v>
+      </c>
+      <c r="H24" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+    </row>
+    <row r="25" spans="1:12" s="7" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="38" t="s">
+      <c r="B25" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="39">
-        <f t="shared" ref="C24" si="15">C20 + 7</f>
+      <c r="C25" s="39">
+        <f t="shared" ref="C25" si="13">C21 + 7</f>
         <v>43031</v>
       </c>
-      <c r="D24" s="40" t="str">
+      <c r="D25" s="40" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Monday</v>
-      </c>
-      <c r="E24" s="41" t="str">
+        <v>понеделник</v>
+      </c>
+      <c r="E25" s="41" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
-        <v>13:30-17:30</v>
-      </c>
-      <c r="F24" s="42" t="str">
+        <v>18:00-22:00</v>
+      </c>
+      <c r="F25" s="42" t="str">
         <f>IF(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), "Team", "Nakov")</f>
         <v>Nakov</v>
       </c>
-      <c r="G24" s="43" t="str">
+      <c r="G25" s="43" t="str">
         <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="H24" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-    </row>
-    <row r="25" spans="1:12" s="7" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="45" t="s">
+      <c r="H25" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="J25" s="49"/>
+      <c r="K25" s="49"/>
+      <c r="L25" s="49"/>
+    </row>
+    <row r="26" spans="1:12" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A26" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="46" t="s">
+      <c r="B26" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="39">
-        <f t="shared" ref="C25" si="16">C24 + 1</f>
+      <c r="C26" s="39">
+        <f t="shared" ref="C26" si="14">C25 + 1</f>
         <v>43032</v>
       </c>
-      <c r="D25" s="40" t="str">
+      <c r="D26" s="40" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Tuesday</v>
-      </c>
-      <c r="E25" s="41" t="str">
+        <v>вторник</v>
+      </c>
+      <c r="E26" s="41" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
         <v>18:00-22:00</v>
       </c>
-      <c r="F25" s="42" t="str">
+      <c r="F26" s="42" t="str">
         <f>IF(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), "Team", "Nakov")</f>
         <v>Team</v>
       </c>
-      <c r="G25" s="43">
+      <c r="G26" s="43">
         <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
-        <v>43038</v>
-      </c>
-      <c r="H25" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="I25" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="J25" s="44"/>
-      <c r="K25" s="44"/>
-      <c r="L25" s="44"/>
-    </row>
-    <row r="26" spans="1:12" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="39">
-        <f t="shared" ref="C26" si="17">C24 + 3</f>
-        <v>43034</v>
-      </c>
-      <c r="D26" s="40" t="str">
-        <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Thursday</v>
-      </c>
-      <c r="E26" s="41" t="str">
-        <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
-        <v>13:30-17:30</v>
-      </c>
-      <c r="F26" s="42" t="str">
-        <f>IF(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), "Team", "Nakov")</f>
-        <v>Nakov</v>
-      </c>
-      <c r="G26" s="43" t="str">
-        <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
-        <v>N/A</v>
+        <v>42866</v>
       </c>
       <c r="H26" s="42" t="s">
         <v>15</v>
       </c>
       <c r="I26" s="42" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J26" s="44"/>
       <c r="K26" s="44"/>
       <c r="L26" s="44"/>
     </row>
     <row r="27" spans="1:12" s="7" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="45" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="46" t="s">
-        <v>64</v>
+      <c r="A27" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="38" t="s">
+        <v>62</v>
       </c>
       <c r="C27" s="39">
-        <f t="shared" ref="C27" si="18">C24 + 4</f>
-        <v>43035</v>
+        <f t="shared" ref="C27" si="15">C25 + 3</f>
+        <v>43034</v>
       </c>
       <c r="D27" s="40" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Friday</v>
+        <v>четвъртък</v>
       </c>
       <c r="E27" s="41" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
@@ -2822,47 +2857,48 @@
       </c>
       <c r="F27" s="42" t="str">
         <f>IF(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), "Team", "Nakov")</f>
-        <v>Team</v>
-      </c>
-      <c r="G27" s="43">
+        <v>Nakov</v>
+      </c>
+      <c r="G27" s="43" t="str">
         <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
-        <v>43041</v>
+        <v>N/A</v>
       </c>
       <c r="H27" s="42" t="s">
         <v>15</v>
       </c>
       <c r="I27" s="42" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J27" s="44"/>
       <c r="K27" s="44"/>
       <c r="L27" s="44"/>
     </row>
     <row r="28" spans="1:12" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="47" t="s">
-        <v>65</v>
-      </c>
-      <c r="B28" s="50" t="s">
-        <v>66</v>
+      <c r="A28" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="46" t="s">
+        <v>64</v>
       </c>
       <c r="C28" s="39">
-        <f t="shared" ref="C28" si="19">C24 + 7</f>
-        <v>43038</v>
+        <f t="shared" ref="C28" si="16">C25 + 4</f>
+        <v>43035</v>
       </c>
       <c r="D28" s="40" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Monday</v>
+        <v>петък</v>
       </c>
       <c r="E28" s="41" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
-        <v>13:30-17:30</v>
-      </c>
-      <c r="F28" s="51" t="s">
-        <v>67</v>
+        <v>18:00-22:00</v>
+      </c>
+      <c r="F28" s="42" t="str">
+        <f>IF(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), "Team", "Nakov")</f>
+        <v>Team</v>
       </c>
       <c r="G28" s="43">
         <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
-        <v>43044</v>
+        <v>42866</v>
       </c>
       <c r="H28" s="42" t="s">
         <v>15</v>
@@ -2876,30 +2912,29 @@
     </row>
     <row r="29" spans="1:12" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A29" s="47" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B29" s="50" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C29" s="39">
-        <f t="shared" ref="C29" si="20">C28 + 1</f>
-        <v>43039</v>
+        <f t="shared" ref="C29" si="17">C25 + 7</f>
+        <v>43038</v>
       </c>
       <c r="D29" s="40" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Tuesday</v>
+        <v>понеделник</v>
       </c>
       <c r="E29" s="41" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
         <v>18:00-22:00</v>
       </c>
-      <c r="F29" s="51" t="str">
-        <f>IF(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), "Team", "TBA")</f>
-        <v>TBA</v>
+      <c r="F29" s="51" t="s">
+        <v>67</v>
       </c>
       <c r="G29" s="43">
         <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
-        <v>43044</v>
+        <v>42866</v>
       </c>
       <c r="H29" s="42" t="s">
         <v>15</v>
@@ -2913,29 +2948,30 @@
     </row>
     <row r="30" spans="1:12" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A30" s="47" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B30" s="50" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C30" s="39">
-        <f t="shared" ref="C30" si="21">C28 + 3</f>
-        <v>43041</v>
+        <f t="shared" ref="C30" si="18">C29 + 1</f>
+        <v>43039</v>
       </c>
       <c r="D30" s="40" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Thursday</v>
+        <v>вторник</v>
       </c>
       <c r="E30" s="41" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
-        <v>13:30-17:30</v>
-      </c>
-      <c r="F30" s="51" t="s">
-        <v>67</v>
+        <v>18:00-22:00</v>
+      </c>
+      <c r="F30" s="51" t="str">
+        <f>IF(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), "Team", "TBA")</f>
+        <v>TBA</v>
       </c>
       <c r="G30" s="43">
         <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
-        <v>43044</v>
+        <v>42866</v>
       </c>
       <c r="H30" s="42" t="s">
         <v>15</v>
@@ -2949,60 +2985,56 @@
     </row>
     <row r="31" spans="1:12" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A31" s="47" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B31" s="50" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C31" s="39">
-        <v>43044</v>
+        <f t="shared" ref="C31" si="19">C29 + 3</f>
+        <v>43041</v>
       </c>
       <c r="D31" s="40" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>Sunday</v>
-      </c>
-      <c r="E31" s="41" t="s">
-        <v>74</v>
+        <v>четвъртък</v>
+      </c>
+      <c r="E31" s="41" t="str">
+        <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
+        <v>18:00-22:00</v>
       </c>
       <c r="F31" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="G31" s="43" t="str">
+      <c r="G31" s="43">
         <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
-        <v>N/A</v>
+        <v>42866</v>
       </c>
       <c r="H31" s="42" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I31" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="J31" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="K31" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="L31" s="44" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="J31" s="44"/>
+      <c r="K31" s="44"/>
+      <c r="L31" s="44"/>
+    </row>
+    <row r="32" spans="1:12" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A32" s="47" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B32" s="50" t="s">
-        <v>79</v>
-      </c>
-      <c r="C32" s="39" t="s">
-        <v>80</v>
+        <v>73</v>
+      </c>
+      <c r="C32" s="39">
+        <v>43044</v>
       </c>
       <c r="D32" s="40" t="str">
         <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
-        <v>TBA</v>
+        <v>неделя</v>
       </c>
       <c r="E32" s="41" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F32" s="51" t="s">
         <v>67</v>
@@ -3011,15 +3043,55 @@
         <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="H32" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="I32" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="J32" s="44"/>
-      <c r="K32" s="44"/>
-      <c r="L32" s="44"/>
+      <c r="H32" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="I32" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="J32" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="K32" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="L32" s="44" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="40" t="str">
+        <f>TEXT(Table2[[#This Row],[Date]],"dddd")</f>
+        <v>TBA</v>
+      </c>
+      <c r="E33" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="F33" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="G33" s="43" t="str">
+        <f>IF(OR(ISNUMBER(SEARCH("Exercises", Table2[[#This Row],[Lesson]])), ISNUMBER(SEARCH("Preparation", Table2[[#This Row],[Lesson]]))), MIN(Table2[[#This Row],[Date]] + 6, "11/5/2017"), "N/A")</f>
+        <v>N/A</v>
+      </c>
+      <c r="H33" s="51" t="s">
+        <v>20</v>
+      </c>
+      <c r="I33" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="J33" s="44"/>
+      <c r="K33" s="44"/>
+      <c r="L33" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3968,7 +4040,7 @@
       </c>
       <c r="E28" s="24" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
-        <v>13:30-17:30</v>
+        <v>18:00-22:00</v>
       </c>
       <c r="F28" s="18" t="s">
         <v>67</v>
@@ -4034,7 +4106,7 @@
       </c>
       <c r="E30" s="24" t="str">
         <f>IF(OR(Table2[[#This Row],[Day]]="Monday", Table2[[#This Row],[Day]]="Thursday"),"13:30-17:30","18:00-22:00")</f>
-        <v>13:30-17:30</v>
+        <v>18:00-22:00</v>
       </c>
       <c r="F30" s="18" t="s">
         <v>67</v>

</xml_diff>